<commit_message>
set booking example date to 2026
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9007F6F-931C-4296-8C71-E1D824CAD8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567FE238-91DB-45F9-8743-1C85C59D2728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="63360" yWindow="3870" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="2844" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,7 +475,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2">
-        <v>45371</v>
+        <v>46101</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -513,7 +513,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="2">
-        <v>45372</v>
+        <v>46102</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update bookings: 2/16/2026, 5:18:24 PM - 7 total bookings
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -630,9 +630,85 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-841107</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-02-19</v>
+      </c>
+      <c r="C7" t="str">
+        <v>test2</v>
+      </c>
+      <c r="D7" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>12134-34345</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H7">
+        <v>32000</v>
+      </c>
+      <c r="I7">
+        <v>32000</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SNOW-841107</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C8" t="str">
+        <v>test2</v>
+      </c>
+      <c r="D8" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E8" t="str">
+        <v>12134-34345</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H8">
+        <v>32000</v>
+      </c>
+      <c r="I8">
+        <v>32000</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update bookings: 2/16/2026, 6:19:34 PM - 5 total bookings
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,104 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E309F0CE-4C1A-4F72-BCB9-37130FBD8DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="4968" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>2026-03-20</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>2026-03-21</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -467,87 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.8984375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-03-20</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -555,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -593,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -631,33 +544,95 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-233683</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="C5" t="str">
+        <v>test</v>
+      </c>
+      <c r="D5" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>123-45567</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H5">
+        <v>18500</v>
+      </c>
+      <c r="I5">
+        <v>18500</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-233683</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="C6" t="str">
+        <v>test</v>
+      </c>
+      <c r="D6" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>123-45567</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H6">
+        <v>18500</v>
+      </c>
+      <c r="I6">
+        <v>18500</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 6 total bookings - 2/16/2026, 7:11:04 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -630,9 +630,47 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-777038</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-02-20</v>
+      </c>
+      <c r="C7" t="str">
+        <v>test</v>
+      </c>
+      <c r="D7" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>1213454</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H7">
+        <v>32000</v>
+      </c>
+      <c r="I7">
+        <v>32000</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update bookings: 5 total bookings - 2/16/2026, 8:08:36 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,104 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFCE3AF-D904-4377-B0CE-4D4554E164F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="3828" yWindow="948" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>2026-03-20</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>2026-03-21</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -467,87 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.8984375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-03-20</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -555,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -593,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -631,32 +544,95 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-772923</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="C5" t="str">
+        <v>test</v>
+      </c>
+      <c r="D5" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>12-34</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H5">
+        <v>32000</v>
+      </c>
+      <c r="I5">
+        <v>32000</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-772923</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="C6" t="str">
+        <v>test</v>
+      </c>
+      <c r="D6" t="str">
+        <v>test@test.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>12-34</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H6">
+        <v>32000</v>
+      </c>
+      <c r="I6">
+        <v>32000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update Bookings: 5 new records (merged with existing data)
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,107 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15F8767-6B26-4A65-AAAB-1659FCF5D276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="3828" yWindow="948" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>2026-03-20</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>2026-03-21</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -470,78 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-03-20</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -549,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -587,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -625,39 +544,57 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="L6" t="s">
-        <v>24</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-779274</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="C5" t="str">
+        <v>test</v>
+      </c>
+      <c r="D5" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>12-23.32434</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H5">
+        <v>18500</v>
+      </c>
+      <c r="I5">
+        <v>18500</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2026-02-16</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L4 L5:L6" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L5"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 5 total bookings - 2/17/2026, 1:15:08 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,104 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8465236-2E19-40B7-B9F1-D7EAC9B78870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>2026-03-20</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>2026-03-21</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -467,78 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-03-20</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -546,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -584,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -622,30 +544,95 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-873775</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="C5" t="str">
+        <v>a</v>
+      </c>
+      <c r="D5" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>12134</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H5">
+        <v>32000</v>
+      </c>
+      <c r="I5">
+        <v>32000</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-873775</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="C6" t="str">
+        <v>a</v>
+      </c>
+      <c r="D6" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>12134</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H6">
+        <v>32000</v>
+      </c>
+      <c r="I6">
+        <v>32000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 7 total bookings - 2/17/2026, 1:36:33 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -630,9 +630,85 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-744415</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-03-19</v>
+      </c>
+      <c r="C7" t="str">
+        <v>march</v>
+      </c>
+      <c r="D7" t="str">
+        <v>m@b.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>1213</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H7">
+        <v>18500</v>
+      </c>
+      <c r="I7">
+        <v>18500</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SNOW-744415</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-03-20</v>
+      </c>
+      <c r="C8" t="str">
+        <v>march</v>
+      </c>
+      <c r="D8" t="str">
+        <v>m@b.com</v>
+      </c>
+      <c r="E8" t="str">
+        <v>1213</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H8">
+        <v>18500</v>
+      </c>
+      <c r="I8">
+        <v>18500</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update bookings: 5 total bookings - 2/17/2026, 2:13:00 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,104 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F57332-04A8-41E4-9CD9-0CC155D234DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="37260" yWindow="1770" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>2026-03-20</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>2026-03-21</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -467,78 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>2026-03-20</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -546,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -584,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2026-03-21</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -622,33 +544,95 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-479585</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="C5" t="str">
+        <v>test</v>
+      </c>
+      <c r="D5" t="str">
+        <v>test@t.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>1213</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H5">
+        <v>32000</v>
+      </c>
+      <c r="I5">
+        <v>64000</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K5" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-479585</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="C6" t="str">
+        <v>test</v>
+      </c>
+      <c r="D6" t="str">
+        <v>test@t.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>1213</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H6">
+        <v>32000</v>
+      </c>
+      <c r="I6">
+        <v>64000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 7 total bookings - 2/17/2026, 2:31:22 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -630,9 +630,85 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-145448</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-02-21</v>
+      </c>
+      <c r="C7" t="str">
+        <v>a</v>
+      </c>
+      <c r="D7" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Weekend Getaway</v>
+      </c>
+      <c r="H7">
+        <v>12800</v>
+      </c>
+      <c r="I7">
+        <v>25600</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SNOW-145448</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-02-22</v>
+      </c>
+      <c r="C8" t="str">
+        <v>a</v>
+      </c>
+      <c r="D8" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E8" t="str">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Weekend Getaway</v>
+      </c>
+      <c r="H8">
+        <v>12800</v>
+      </c>
+      <c r="I8">
+        <v>25600</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2026-02-17</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update bookings: 6 total bookings - 2/17/2026, 3:25:21 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,104 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1F8A7C-3E13-43FD-83E9-3F1849A9AFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="30495" yWindow="1815" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>SNOW-004</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,23 +64,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -468,77 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
-        <v>46102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>16</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -546,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>18</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1">
-        <v>46102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -584,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>17</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>18</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1">
-        <v>46102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>16</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -622,37 +544,37 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>18</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1">
-        <v>46079</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2/26/2026</v>
+      </c>
+      <c r="C5" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D5" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>16</v>
+      <c r="G5" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H5">
         <v>12800</v>
@@ -660,35 +582,95 @@
       <c r="I5">
         <v>12800</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K5">
         <v>45352</v>
       </c>
-      <c r="L5" t="s">
-        <v>18</v>
+      <c r="L5" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="L6" t="s">
-        <v>22</v>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-497850</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2/22/2026</v>
+      </c>
+      <c r="C6" t="str">
+        <v>a</v>
+      </c>
+      <c r="D6" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>1231213</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H6">
+        <v>32000</v>
+      </c>
+      <c r="I6">
+        <v>64000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2/17/2026</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-497850</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="C7" t="str">
+        <v>a</v>
+      </c>
+      <c r="D7" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>1231213</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H7">
+        <v>32000</v>
+      </c>
+      <c r="I7">
+        <v>64000</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2/17/2026</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L1 L6 A4 A2 C2:L2 A3 C3:L3 C4:L4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
add faster resynch from excel to calendar
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1F8A7C-3E13-43FD-83E9-3F1849A9AFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7341A89E-37BD-4FA5-9FDD-6CF6DC3BE1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30495" yWindow="1815" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30060" yWindow="1380" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -523,7 +523,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="1">
-        <v>46102</v>
+        <v>46101</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Update bookings: 7 total bookings - 2/23/2026, 11:57:35 AM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,104 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F76CAFF-A3EC-4AAC-AC71-02EBDE43A3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>SNOW-004</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,23 +64,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -468,78 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.09765625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
-        <v>46101</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>3/20/2026</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>16</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -547,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>18</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1">
-        <v>46102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>16</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -585,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>17</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>18</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1">
-        <v>46102</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>16</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -623,37 +544,37 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>18</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1">
-        <v>46107</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>3/26/2026</v>
+      </c>
+      <c r="C5" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D5" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>16</v>
+      <c r="G5" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H5">
         <v>12800</v>
@@ -661,35 +582,133 @@
       <c r="I5">
         <v>12800</v>
       </c>
-      <c r="J5" t="s">
-        <v>17</v>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K5">
         <v>45352</v>
       </c>
-      <c r="L5" t="s">
-        <v>18</v>
+      <c r="L5" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="L6" t="s">
-        <v>22</v>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-631313</v>
+      </c>
+      <c r="B6" t="str">
+        <v>3/18/2026</v>
+      </c>
+      <c r="C6" t="str">
+        <v>test</v>
+      </c>
+      <c r="D6" t="str">
+        <v>test@t.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>121324</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H6">
+        <v>32000</v>
+      </c>
+      <c r="I6">
+        <v>96000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-631313</v>
+      </c>
+      <c r="B7" t="str">
+        <v>3/19/2026</v>
+      </c>
+      <c r="C7" t="str">
+        <v>test</v>
+      </c>
+      <c r="D7" t="str">
+        <v>test@t.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>121324</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H7">
+        <v>32000</v>
+      </c>
+      <c r="I7">
+        <v>96000</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SNOW-631313</v>
+      </c>
+      <c r="B8" t="str">
+        <v>3/20/2026</v>
+      </c>
+      <c r="C8" t="str">
+        <v>test</v>
+      </c>
+      <c r="D8" t="str">
+        <v>test@t.com</v>
+      </c>
+      <c r="E8" t="str">
+        <v>121324</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H8">
+        <v>32000</v>
+      </c>
+      <c r="I8">
+        <v>96000</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L1 L6 A4 A2 C2:L2 A3 C3:L3 C4:L4" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 5 total bookings - 2/23/2026, 1:32:54 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,110 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51235621-FFB0-49DD-A15F-8E62B363217C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>3/20/2026</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>3/21/2026</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-  <si>
-    <t>SNOW-004</t>
-  </si>
-  <si>
-    <t>3/26/2026</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -473,74 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>3/20/2026</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -548,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -586,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -624,37 +544,37 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>3/26/2026</v>
+      </c>
+      <c r="C5" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D5" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
+      <c r="G5" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H5">
         <v>12800</v>
@@ -662,32 +582,57 @@
       <c r="I5">
         <v>12800</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K5">
         <v>45352</v>
       </c>
-      <c r="L5" t="s">
-        <v>19</v>
+      <c r="L5" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-748026</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2/24/2026</v>
+      </c>
+      <c r="C6" t="str">
+        <v>test</v>
+      </c>
+      <c r="D6" t="str">
+        <v>est@t.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>123</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H6">
+        <v>32000</v>
+      </c>
+      <c r="I6">
+        <v>32000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L5" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 7 total bookings - 2/23/2026, 3:26:42 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -630,9 +630,85 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-745596</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2026-02-26</v>
+      </c>
+      <c r="C7" t="str">
+        <v>local</v>
+      </c>
+      <c r="D7" t="str">
+        <v>loca@a.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>1212</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H7">
+        <v>32000</v>
+      </c>
+      <c r="I7">
+        <v>64000</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SNOW-745596</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2026-02-27</v>
+      </c>
+      <c r="C8" t="str">
+        <v>local</v>
+      </c>
+      <c r="D8" t="str">
+        <v>loca@a.com</v>
+      </c>
+      <c r="E8" t="str">
+        <v>1212</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H8">
+        <v>32000</v>
+      </c>
+      <c r="I8">
+        <v>64000</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2026-02-23</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update bookings: 9 total bookings - 2/23/2026, 3:30:10 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -706,9 +706,85 @@
         <v/>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>SNOW-355489</v>
+      </c>
+      <c r="B9" t="str">
+        <v>2/24/2026</v>
+      </c>
+      <c r="C9" t="str">
+        <v>a</v>
+      </c>
+      <c r="D9" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E9" t="str">
+        <v>swee3</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H9">
+        <v>32000</v>
+      </c>
+      <c r="I9">
+        <v>64000</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K9" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>SNOW-355489</v>
+      </c>
+      <c r="B10" t="str">
+        <v>2/25/2026</v>
+      </c>
+      <c r="C10" t="str">
+        <v>a</v>
+      </c>
+      <c r="D10" t="str">
+        <v>a@b.com</v>
+      </c>
+      <c r="E10" t="str">
+        <v>swee3</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H10">
+        <v>32000</v>
+      </c>
+      <c r="I10">
+        <v>64000</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K10" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L10" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update bookings: 6 total bookings - 2/23/2026, 3:57:44 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,110 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45980FF-C254-411C-BB97-B9EB1E5D1B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>3/20/2026</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>3/21/2026</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-  <si>
-    <t>SNOW-004</t>
-  </si>
-  <si>
-    <t>3/26/2026</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -473,77 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>3/20/2026</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -551,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -589,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -627,37 +544,37 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>3/26/2026</v>
+      </c>
+      <c r="C5" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D5" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
+      <c r="G5" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H5">
         <v>12800</v>
@@ -665,34 +582,95 @@
       <c r="I5">
         <v>12800</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K5">
         <v>45352</v>
       </c>
-      <c r="L5" t="s">
-        <v>19</v>
+      <c r="L5" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-357602</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2/24/2026</v>
+      </c>
+      <c r="C6" t="str">
+        <v>desktop</v>
+      </c>
+      <c r="D6" t="str">
+        <v>d@d.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>223</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H6">
+        <v>18500</v>
+      </c>
+      <c r="I6">
+        <v>37000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-357602</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2/25/2026</v>
+      </c>
+      <c r="C7" t="str">
+        <v>desktop</v>
+      </c>
+      <c r="D7" t="str">
+        <v>d@d.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>223</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H7">
+        <v>18500</v>
+      </c>
+      <c r="I7">
+        <v>37000</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L5" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 6 total bookings - 2/23/2026, 3:59:44 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -594,31 +594,31 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>SNOW-357602</v>
+        <v>SNOW-712162</v>
       </c>
       <c r="B6" t="str">
-        <v>2/24/2026</v>
+        <v>2/26/2026</v>
       </c>
       <c r="C6" t="str">
-        <v>desktop</v>
+        <v>local</v>
       </c>
       <c r="D6" t="str">
-        <v>d@d.com</v>
+        <v>l@l.com</v>
       </c>
       <c r="E6" t="str">
-        <v>223</v>
+        <v>323</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="str">
-        <v>Ski Adventure</v>
+        <v>Family Ski Package</v>
       </c>
       <c r="H6">
-        <v>18500</v>
+        <v>32000</v>
       </c>
       <c r="I6">
-        <v>37000</v>
+        <v>64000</v>
       </c>
       <c r="J6" t="str">
         <v>Confirmed</v>
@@ -632,31 +632,31 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>SNOW-357602</v>
+        <v>SNOW-712162</v>
       </c>
       <c r="B7" t="str">
-        <v>2/25/2026</v>
+        <v>2/27/2026</v>
       </c>
       <c r="C7" t="str">
-        <v>desktop</v>
+        <v>local</v>
       </c>
       <c r="D7" t="str">
-        <v>d@d.com</v>
+        <v>l@l.com</v>
       </c>
       <c r="E7" t="str">
-        <v>223</v>
+        <v>323</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="str">
-        <v>Ski Adventure</v>
+        <v>Family Ski Package</v>
       </c>
       <c r="H7">
-        <v>18500</v>
+        <v>32000</v>
       </c>
       <c r="I7">
-        <v>37000</v>
+        <v>64000</v>
       </c>
       <c r="J7" t="str">
         <v>Confirmed</v>

</xml_diff>

<commit_message>
Update bookings: 5 total bookings - 2/23/2026, 4:09:46 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -1,110 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Calendar\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05814A0-85D8-43F4-8F19-7647D0992070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Bookings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
-  <si>
-    <t>Booking ID</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Customer Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Guests</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Plan Price</t>
-  </si>
-  <si>
-    <t>Total Price</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Booking Date</t>
-  </si>
-  <si>
-    <t>Special Requests</t>
-  </si>
-  <si>
-    <t>SNOW-001</t>
-  </si>
-  <si>
-    <t>3/20/2026</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@email.com</t>
-  </si>
-  <si>
-    <t>555-0101</t>
-  </si>
-  <si>
-    <t>Weekend Getaway</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>Late check-in requested</t>
-  </si>
-  <si>
-    <t>SNOW-002</t>
-  </si>
-  <si>
-    <t>3/21/2026</t>
-  </si>
-  <si>
-    <t>SNOW-003</t>
-  </si>
-  <si>
-    <t>John Smith2</t>
-  </si>
-  <si>
-    <t>SNOW-004</t>
-  </si>
-  <si>
-    <t>3/26/2026</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,14 +72,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -473,79 +396,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:M12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Booking ID</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Customer Name</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Email</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Guests</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Plan</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Plan Price</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Total Price</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Status</v>
+      </c>
+      <c r="K1" t="str">
+        <v>Booking Date</v>
+      </c>
+      <c r="L1" t="str">
+        <v>Special Requests</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>SNOW-001</v>
+      </c>
+      <c r="B2" t="str">
+        <v>3/20/2026</v>
+      </c>
+      <c r="C2" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D2" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E2" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>17</v>
+      <c r="G2" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H2">
         <v>12800</v>
@@ -553,37 +468,37 @@
       <c r="I2">
         <v>12800</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
+      <c r="J2" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K2">
         <v>45352</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
+      <c r="L2" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>SNOW-002</v>
+      </c>
+      <c r="B3" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C3" t="str">
+        <v>John Smith</v>
+      </c>
+      <c r="D3" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E3" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>17</v>
+      <c r="G3" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H3">
         <v>12800</v>
@@ -591,37 +506,37 @@
       <c r="I3">
         <v>12800</v>
       </c>
-      <c r="J3" t="s">
-        <v>18</v>
+      <c r="J3" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K3">
         <v>45352</v>
       </c>
-      <c r="L3" t="s">
-        <v>19</v>
+      <c r="L3" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>SNOW-003</v>
+      </c>
+      <c r="B4" t="str">
+        <v>3/21/2026</v>
+      </c>
+      <c r="C4" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D4" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E4" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>17</v>
+      <c r="G4" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H4">
         <v>12800</v>
@@ -629,37 +544,37 @@
       <c r="I4">
         <v>12800</v>
       </c>
-      <c r="J4" t="s">
-        <v>18</v>
+      <c r="J4" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K4">
         <v>45352</v>
       </c>
-      <c r="L4" t="s">
-        <v>19</v>
+      <c r="L4" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>SNOW-004</v>
+      </c>
+      <c r="B5" t="str">
+        <v>3/26/2026</v>
+      </c>
+      <c r="C5" t="str">
+        <v>John Smith2</v>
+      </c>
+      <c r="D5" t="str">
+        <v>john@email.com</v>
+      </c>
+      <c r="E5" t="str">
+        <v>555-0101</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
+      <c r="G5" t="str">
+        <v>Weekend Getaway</v>
       </c>
       <c r="H5">
         <v>12800</v>
@@ -667,31 +582,57 @@
       <c r="I5">
         <v>12800</v>
       </c>
-      <c r="J5" t="s">
-        <v>18</v>
+      <c r="J5" t="str">
+        <v>Confirmed</v>
       </c>
       <c r="K5">
         <v>45352</v>
       </c>
-      <c r="L5" t="s">
-        <v>19</v>
+      <c r="L5" t="str">
+        <v>Late check-in requested</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>SNOW-675941</v>
+      </c>
+      <c r="B6" t="str">
+        <v>2/24/2026</v>
+      </c>
+      <c r="C6" t="str">
+        <v>desk</v>
+      </c>
+      <c r="D6" t="str">
+        <v>d@d.com</v>
+      </c>
+      <c r="E6" t="str">
+        <v>desk</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>Ski Adventure</v>
+      </c>
+      <c r="H6">
+        <v>18500</v>
+      </c>
+      <c r="I6">
+        <v>18500</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K6" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L6" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Internal</oddFooter>
-  </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="A1:L5" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
-<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{7e753c2c-bb14-4786-921b-97c6a6fc424f}" enabled="1" method="Standard" siteId="{3bd97919-57c3-48d3-9e9a-8e4c01614a8f}" contentBits="2" removed="0"/>
-</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Update bookings: 6 total bookings - 2/23/2026, 4:15:22 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -630,9 +630,47 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>SNOW-401902</v>
+      </c>
+      <c r="B7" t="str">
+        <v>2/25/2026</v>
+      </c>
+      <c r="C7" t="str">
+        <v>local</v>
+      </c>
+      <c r="D7" t="str">
+        <v>l@l.com</v>
+      </c>
+      <c r="E7" t="str">
+        <v>local1231</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>Family Ski Package</v>
+      </c>
+      <c r="H7">
+        <v>32000</v>
+      </c>
+      <c r="I7">
+        <v>32000</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K7" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update bookings: 7 total bookings - 2/23/2026, 4:37:04 PM
</commit_message>
<xml_diff>
--- a/data/calendar-bookings.xlsx
+++ b/data/calendar-bookings.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -668,9 +668,47 @@
         <v/>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>SNOW-773795</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2/26/2026</v>
+      </c>
+      <c r="C8" t="str">
+        <v>desk</v>
+      </c>
+      <c r="D8" t="str">
+        <v>d@d.com</v>
+      </c>
+      <c r="E8" t="str">
+        <v>d</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <v>Weekend Getaway</v>
+      </c>
+      <c r="H8">
+        <v>12800</v>
+      </c>
+      <c r="I8">
+        <v>12800</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Confirmed</v>
+      </c>
+      <c r="K8" t="str">
+        <v>2/23/2026</v>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>